<commit_message>
more updates to great schools
</commit_message>
<xml_diff>
--- a/public_school_data.xlsx
+++ b/public_school_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="495">
   <si>
     <t>Rating</t>
   </si>
@@ -508,6 +508,132 @@
     <t>St. Francis High School</t>
   </si>
   <si>
+    <t>Frost Lake Magnet Elementary School</t>
+  </si>
+  <si>
+    <t>Parkway Montessori/Community Middle</t>
+  </si>
+  <si>
+    <t>Johnson Senior High School</t>
+  </si>
+  <si>
+    <t>Washington Elementary School</t>
+  </si>
+  <si>
+    <t>Mankato East Jr.</t>
+  </si>
+  <si>
+    <t>Mankato East Senior High School</t>
+  </si>
+  <si>
+    <t>Paul A. Smith School</t>
+  </si>
+  <si>
+    <t>Franklin Middle School</t>
+  </si>
+  <si>
+    <t>Franklin High School</t>
+  </si>
+  <si>
+    <t>Kawameeh Middle School</t>
+  </si>
+  <si>
+    <t>Union Senior High School</t>
+  </si>
+  <si>
+    <t>Creekside Elementary School</t>
+  </si>
+  <si>
+    <t>A G Cox Middle School</t>
+  </si>
+  <si>
+    <t>South Central High School</t>
+  </si>
+  <si>
+    <t>Holt Elementary Language Academy</t>
+  </si>
+  <si>
+    <t>George L Carrington Middle</t>
+  </si>
+  <si>
+    <t>Riverside High School</t>
+  </si>
+  <si>
+    <t>Eastway Elementary</t>
+  </si>
+  <si>
+    <t>Neal Middle</t>
+  </si>
+  <si>
+    <t>Northern High</t>
+  </si>
+  <si>
+    <t>Parkwood Elementary</t>
+  </si>
+  <si>
+    <t>Lowe's Grove Middle</t>
+  </si>
+  <si>
+    <t>Hillside High</t>
+  </si>
+  <si>
+    <t>Youngsville Elementary</t>
+  </si>
+  <si>
+    <t>Cedar Creek Middle</t>
+  </si>
+  <si>
+    <t>Franklinton High</t>
+  </si>
+  <si>
+    <t>Skelly Elementary School</t>
+  </si>
+  <si>
+    <t>Hale Junior High School</t>
+  </si>
+  <si>
+    <t>Nathan Hale High School</t>
+  </si>
+  <si>
+    <t>Marshall Elementary School</t>
+  </si>
+  <si>
+    <t>Memorial Junior High School</t>
+  </si>
+  <si>
+    <t>Memorial High School</t>
+  </si>
+  <si>
+    <t>Obadiah Knight Elementary School</t>
+  </si>
+  <si>
+    <t>Thomas J Rusk Middle School</t>
+  </si>
+  <si>
+    <t>North Dallas High School</t>
+  </si>
+  <si>
+    <t>Academy Elementary School</t>
+  </si>
+  <si>
+    <t>Academy J H</t>
+  </si>
+  <si>
+    <t>Academy High School</t>
+  </si>
+  <si>
+    <t>Anderson Academy</t>
+  </si>
+  <si>
+    <t>Houston Academy</t>
+  </si>
+  <si>
+    <t>Drew Academy</t>
+  </si>
+  <si>
+    <t>Carver High School For Applied Tech/Engine</t>
+  </si>
+  <si>
     <t>11915 Price Road, Hebron, IL, 60034</t>
   </si>
   <si>
@@ -946,6 +1072,135 @@
     <t>3325 Bridge Street Northwest, Saint Francis, MN, 55070</t>
   </si>
   <si>
+    <t>1505 Hoyt Avenue East, Saint Paul, MN, 55106</t>
+  </si>
+  <si>
+    <t>1363 Bush Avenue, Saint Paul, MN, 55106</t>
+  </si>
+  <si>
+    <t>1349 Arcade Street, Saint Paul, MN, 55106</t>
+  </si>
+  <si>
+    <t>1100 Anderson Drive, Mankato, MN, 56001</t>
+  </si>
+  <si>
+    <t>1200 Prairie Winds Drive, Mankato, MN, 56001</t>
+  </si>
+  <si>
+    <t>2600 Hoffman Road, Mankato, MN, 56001</t>
+  </si>
+  <si>
+    <t>41 Daniel Webster Drive, Franklin, NH, 03235</t>
+  </si>
+  <si>
+    <t>200 Sanborn Street, Franklin, NH, 03235</t>
+  </si>
+  <si>
+    <t>115 Central Street, Franklin, NH, 03235</t>
+  </si>
+  <si>
+    <t>301 Washington Avenue, Union, NJ, 07083</t>
+  </si>
+  <si>
+    <t>490 David Terrace, Union, NJ, 07083</t>
+  </si>
+  <si>
+    <t>2350 North 3rd Street, Union, NJ, 07083</t>
+  </si>
+  <si>
+    <t>431 Forlines Road, Winterville, NC, 28590</t>
+  </si>
+  <si>
+    <t>2657 Church Street, Winterville, NC, 28590</t>
+  </si>
+  <si>
+    <t>570 Forlines Road, Winterville, NC, 28590</t>
+  </si>
+  <si>
+    <t>4019 Holt School Road, Durham, NC, 27704</t>
+  </si>
+  <si>
+    <t>227 Milton Road, Durham, NC, 27712</t>
+  </si>
+  <si>
+    <t>3218 Rose of Sharon Road, Durham, NC, 27712</t>
+  </si>
+  <si>
+    <t>610 North Alston Avenue, Durham, NC, 27701</t>
+  </si>
+  <si>
+    <t>201 Baptist Road, Durham, NC, 27704</t>
+  </si>
+  <si>
+    <t>117 Tom Wilkinson Road, Durham, NC, 27712</t>
+  </si>
+  <si>
+    <t>5207 Revere Road, Durham, NC, 27713</t>
+  </si>
+  <si>
+    <t>4418 South Alston Avenue, Durham, NC, 27713</t>
+  </si>
+  <si>
+    <t>3727 Fayetteville Road, Durham, NC, 27707</t>
+  </si>
+  <si>
+    <t>125 HWY 1A South, Youngsville, NC, 27596</t>
+  </si>
+  <si>
+    <t>2228 Cedar Creek Road, Youngsville, NC, 27596</t>
+  </si>
+  <si>
+    <t>910 Cedar Creek Rd, Franklinton, NC, 27525</t>
+  </si>
+  <si>
+    <t>2940 South 90th East Avenue, Tulsa, OK, 74129</t>
+  </si>
+  <si>
+    <t>2177 South 67th East Avenue, Tulsa, OK, 74129</t>
+  </si>
+  <si>
+    <t>6960 East 21st Street, Tulsa, OK, 74129</t>
+  </si>
+  <si>
+    <t>1142 East 56th Street, Tulsa, OK, 74105</t>
+  </si>
+  <si>
+    <t>7502 East 57th Street, Tulsa, OK, 74145</t>
+  </si>
+  <si>
+    <t>5840 South Hudson Avenue, Tulsa, OK, 74135</t>
+  </si>
+  <si>
+    <t>2615 Anson Road, Dallas, TX, 75235</t>
+  </si>
+  <si>
+    <t>2929 Inwood Road, Dallas, TX, 75235</t>
+  </si>
+  <si>
+    <t>3120 North Haskell Avenue, Dallas, TX, 75204</t>
+  </si>
+  <si>
+    <t>107 South Pondalily, Little River-Academy, TX, 76554</t>
+  </si>
+  <si>
+    <t>501 East Main Street, Little River-Academy, TX, 76554</t>
+  </si>
+  <si>
+    <t>602 East Main Street, Little River-Academy, TX, 76554</t>
+  </si>
+  <si>
+    <t>7401 Wheatley Street, Houston, TX, 77088</t>
+  </si>
+  <si>
+    <t>8103 Carver Road, Houston, TX, 77088</t>
+  </si>
+  <si>
+    <t>1910 West Little York Road, Houston, TX, 77091</t>
+  </si>
+  <si>
+    <t>2100 South Victory Drive, Houston, TX, 77088</t>
+  </si>
+  <si>
     <t>Public district</t>
   </si>
   <si>
@@ -1018,6 +1273,15 @@
     <t xml:space="preserve"> 7-12</t>
   </si>
   <si>
+    <t xml:space="preserve"> K-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1-3</t>
+  </si>
+  <si>
     <t>42.4655661-88.43101038</t>
   </si>
   <si>
@@ -1193,6 +1457,48 @@
   </si>
   <si>
     <t>45.40007657-93.37122273</t>
+  </si>
+  <si>
+    <t>44.98965324-93.03668889</t>
+  </si>
+  <si>
+    <t>44.16677076-94.00042</t>
+  </si>
+  <si>
+    <t>43.44248333-71.64721446</t>
+  </si>
+  <si>
+    <t>40.6765569-74.22857306</t>
+  </si>
+  <si>
+    <t>35.54845586-77.40720915</t>
+  </si>
+  <si>
+    <t>36.04728965-78.90046671</t>
+  </si>
+  <si>
+    <t>35.99481799-78.88121936</t>
+  </si>
+  <si>
+    <t>35.9137798-78.90176986</t>
+  </si>
+  <si>
+    <t>36.02233222-78.48781449</t>
+  </si>
+  <si>
+    <t>36.12529979-95.86364364</t>
+  </si>
+  <si>
+    <t>36.0818835-95.97721949</t>
+  </si>
+  <si>
+    <t>32.8352633-96.86735477</t>
+  </si>
+  <si>
+    <t>30.98393892-97.33970241</t>
+  </si>
+  <si>
+    <t>29.86460065-95.44033647</t>
   </si>
 </sst>
 </file>
@@ -1550,7 +1856,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H147"/>
+  <dimension ref="A1:H190"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1590,19 +1896,19 @@
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
       <c r="E2" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F2" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G2">
         <v>217</v>
       </c>
       <c r="H2" t="s">
-        <v>334</v>
+        <v>422</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1616,19 +1922,19 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>165</v>
+        <v>207</v>
       </c>
       <c r="E3" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F3" t="s">
-        <v>313</v>
+        <v>398</v>
       </c>
       <c r="G3">
         <v>495</v>
       </c>
       <c r="H3" t="s">
-        <v>335</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1642,19 +1948,19 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>166</v>
+        <v>208</v>
       </c>
       <c r="E4" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F4" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G4">
         <v>1635</v>
       </c>
       <c r="H4" t="s">
-        <v>335</v>
+        <v>423</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1668,19 +1974,19 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>167</v>
+        <v>209</v>
       </c>
       <c r="E5" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F5" t="s">
-        <v>315</v>
+        <v>400</v>
       </c>
       <c r="G5">
         <v>478</v>
       </c>
       <c r="H5" t="s">
-        <v>336</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1694,19 +2000,19 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="E6" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F6" t="s">
-        <v>316</v>
+        <v>401</v>
       </c>
       <c r="G6">
         <v>738</v>
       </c>
       <c r="H6" t="s">
-        <v>336</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1720,19 +2026,19 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>169</v>
+        <v>211</v>
       </c>
       <c r="E7" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F7" t="s">
-        <v>317</v>
+        <v>402</v>
       </c>
       <c r="G7">
         <v>782</v>
       </c>
       <c r="H7" t="s">
-        <v>336</v>
+        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1746,19 +2052,19 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>170</v>
+        <v>212</v>
       </c>
       <c r="E8" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F8" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G8">
         <v>1560</v>
       </c>
       <c r="H8" t="s">
-        <v>336</v>
+        <v>424</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1772,19 +2078,19 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>171</v>
+        <v>213</v>
       </c>
       <c r="E9" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F9" t="s">
-        <v>313</v>
+        <v>398</v>
       </c>
       <c r="G9">
         <v>548</v>
       </c>
       <c r="H9" t="s">
-        <v>337</v>
+        <v>425</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1798,19 +2104,19 @@
         <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>172</v>
+        <v>214</v>
       </c>
       <c r="E10" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F10" t="s">
-        <v>317</v>
+        <v>402</v>
       </c>
       <c r="G10">
         <v>1018</v>
       </c>
       <c r="H10" t="s">
-        <v>337</v>
+        <v>425</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1824,19 +2130,19 @@
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>173</v>
+        <v>215</v>
       </c>
       <c r="E11" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F11" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G11">
         <v>1624</v>
       </c>
       <c r="H11" t="s">
-        <v>337</v>
+        <v>425</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1850,19 +2156,19 @@
         <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>174</v>
+        <v>216</v>
       </c>
       <c r="E12" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F12" t="s">
-        <v>313</v>
+        <v>398</v>
       </c>
       <c r="G12">
         <v>548</v>
       </c>
       <c r="H12" t="s">
-        <v>338</v>
+        <v>426</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1876,19 +2182,19 @@
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>175</v>
+        <v>217</v>
       </c>
       <c r="E13" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F13" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G13">
         <v>1066</v>
       </c>
       <c r="H13" t="s">
-        <v>338</v>
+        <v>426</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1902,19 +2208,19 @@
         <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>176</v>
+        <v>218</v>
       </c>
       <c r="E14" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F14" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G14">
         <v>645</v>
       </c>
       <c r="H14" t="s">
-        <v>339</v>
+        <v>427</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1928,19 +2234,19 @@
         <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>177</v>
+        <v>219</v>
       </c>
       <c r="E15" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F15" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G15">
         <v>748</v>
       </c>
       <c r="H15" t="s">
-        <v>339</v>
+        <v>427</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1954,19 +2260,19 @@
         <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>178</v>
+        <v>220</v>
       </c>
       <c r="E16" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F16" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G16">
         <v>695</v>
       </c>
       <c r="H16" t="s">
-        <v>340</v>
+        <v>428</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1980,19 +2286,19 @@
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>179</v>
+        <v>221</v>
       </c>
       <c r="E17" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F17" t="s">
-        <v>319</v>
+        <v>404</v>
       </c>
       <c r="G17">
         <v>748</v>
       </c>
       <c r="H17" t="s">
-        <v>340</v>
+        <v>428</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2006,19 +2312,19 @@
         <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>180</v>
+        <v>222</v>
       </c>
       <c r="E18" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F18" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G18">
         <v>1987</v>
       </c>
       <c r="H18" t="s">
-        <v>340</v>
+        <v>428</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2032,19 +2338,19 @@
         <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>181</v>
+        <v>223</v>
       </c>
       <c r="E19" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F19" t="s">
-        <v>320</v>
+        <v>405</v>
       </c>
       <c r="G19">
         <v>630</v>
       </c>
       <c r="H19" t="s">
-        <v>341</v>
+        <v>429</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2058,19 +2364,19 @@
         <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="E20" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F20" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G20">
         <v>1096</v>
       </c>
       <c r="H20" t="s">
-        <v>341</v>
+        <v>429</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2084,19 +2390,19 @@
         <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>183</v>
+        <v>225</v>
       </c>
       <c r="E21" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F21" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G21">
         <v>1801</v>
       </c>
       <c r="H21" t="s">
-        <v>341</v>
+        <v>429</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2110,19 +2416,19 @@
         <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>184</v>
+        <v>226</v>
       </c>
       <c r="E22" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F22" t="s">
-        <v>321</v>
+        <v>406</v>
       </c>
       <c r="G22">
         <v>484</v>
       </c>
       <c r="H22" t="s">
-        <v>342</v>
+        <v>430</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2136,19 +2442,19 @@
         <v>39</v>
       </c>
       <c r="D23" t="s">
-        <v>185</v>
+        <v>227</v>
       </c>
       <c r="E23" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F23" t="s">
-        <v>322</v>
+        <v>407</v>
       </c>
       <c r="G23">
         <v>1261</v>
       </c>
       <c r="H23" t="s">
-        <v>342</v>
+        <v>430</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2162,19 +2468,19 @@
         <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>186</v>
+        <v>228</v>
       </c>
       <c r="E24" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F24" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G24">
         <v>575</v>
       </c>
       <c r="H24" t="s">
-        <v>342</v>
+        <v>430</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2188,19 +2494,19 @@
         <v>41</v>
       </c>
       <c r="D25" t="s">
-        <v>187</v>
+        <v>229</v>
       </c>
       <c r="E25" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F25" t="s">
-        <v>317</v>
+        <v>402</v>
       </c>
       <c r="G25">
         <v>676</v>
       </c>
       <c r="H25" t="s">
-        <v>343</v>
+        <v>431</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2214,19 +2520,19 @@
         <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>188</v>
+        <v>230</v>
       </c>
       <c r="E26" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F26" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G26">
         <v>2720</v>
       </c>
       <c r="H26" t="s">
-        <v>343</v>
+        <v>431</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2240,19 +2546,19 @@
         <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>189</v>
+        <v>231</v>
       </c>
       <c r="E27" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F27" t="s">
-        <v>321</v>
+        <v>406</v>
       </c>
       <c r="G27">
         <v>582</v>
       </c>
       <c r="H27" t="s">
-        <v>344</v>
+        <v>432</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2266,19 +2572,19 @@
         <v>44</v>
       </c>
       <c r="D28" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="E28" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F28" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G28">
         <v>949</v>
       </c>
       <c r="H28" t="s">
-        <v>344</v>
+        <v>432</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2292,19 +2598,19 @@
         <v>45</v>
       </c>
       <c r="D29" t="s">
-        <v>191</v>
+        <v>233</v>
       </c>
       <c r="E29" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F29" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G29">
         <v>2531</v>
       </c>
       <c r="H29" t="s">
-        <v>344</v>
+        <v>432</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2318,19 +2624,19 @@
         <v>46</v>
       </c>
       <c r="D30" t="s">
-        <v>192</v>
+        <v>234</v>
       </c>
       <c r="E30" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F30" t="s">
-        <v>323</v>
+        <v>408</v>
       </c>
       <c r="G30">
         <v>314</v>
       </c>
       <c r="H30" t="s">
-        <v>345</v>
+        <v>433</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2344,19 +2650,19 @@
         <v>47</v>
       </c>
       <c r="D31" t="s">
-        <v>193</v>
+        <v>235</v>
       </c>
       <c r="E31" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F31" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G31">
         <v>231</v>
       </c>
       <c r="H31" t="s">
-        <v>345</v>
+        <v>433</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2370,19 +2676,19 @@
         <v>48</v>
       </c>
       <c r="D32" t="s">
-        <v>194</v>
+        <v>236</v>
       </c>
       <c r="E32" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F32" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G32">
         <v>835</v>
       </c>
       <c r="H32" t="s">
-        <v>345</v>
+        <v>433</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2396,19 +2702,19 @@
         <v>49</v>
       </c>
       <c r="D33" t="s">
-        <v>195</v>
+        <v>237</v>
       </c>
       <c r="E33" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F33" t="s">
-        <v>321</v>
+        <v>406</v>
       </c>
       <c r="G33">
         <v>194</v>
       </c>
       <c r="H33" t="s">
-        <v>346</v>
+        <v>434</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2422,19 +2728,19 @@
         <v>50</v>
       </c>
       <c r="D34" t="s">
-        <v>196</v>
+        <v>238</v>
       </c>
       <c r="E34" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F34" t="s">
-        <v>321</v>
+        <v>406</v>
       </c>
       <c r="G34">
         <v>795</v>
       </c>
       <c r="H34" t="s">
-        <v>347</v>
+        <v>435</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2448,19 +2754,19 @@
         <v>51</v>
       </c>
       <c r="D35" t="s">
-        <v>197</v>
+        <v>239</v>
       </c>
       <c r="E35" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F35" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G35">
         <v>926</v>
       </c>
       <c r="H35" t="s">
-        <v>347</v>
+        <v>435</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2474,19 +2780,19 @@
         <v>52</v>
       </c>
       <c r="D36" t="s">
-        <v>198</v>
+        <v>240</v>
       </c>
       <c r="E36" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F36" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G36">
         <v>2523</v>
       </c>
       <c r="H36" t="s">
-        <v>347</v>
+        <v>435</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2500,19 +2806,19 @@
         <v>53</v>
       </c>
       <c r="D37" t="s">
-        <v>199</v>
+        <v>241</v>
       </c>
       <c r="E37" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F37" t="s">
-        <v>321</v>
+        <v>406</v>
       </c>
       <c r="G37">
         <v>587</v>
       </c>
       <c r="H37" t="s">
-        <v>348</v>
+        <v>436</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2526,19 +2832,19 @@
         <v>54</v>
       </c>
       <c r="D38" t="s">
-        <v>200</v>
+        <v>242</v>
       </c>
       <c r="E38" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F38" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G38">
         <v>1157</v>
       </c>
       <c r="H38" t="s">
-        <v>348</v>
+        <v>436</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2552,19 +2858,19 @@
         <v>55</v>
       </c>
       <c r="D39" t="s">
-        <v>201</v>
+        <v>243</v>
       </c>
       <c r="E39" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F39" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G39">
         <v>1723</v>
       </c>
       <c r="H39" t="s">
-        <v>348</v>
+        <v>436</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2578,19 +2884,19 @@
         <v>56</v>
       </c>
       <c r="D40" t="s">
-        <v>202</v>
+        <v>244</v>
       </c>
       <c r="E40" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F40" t="s">
-        <v>321</v>
+        <v>406</v>
       </c>
       <c r="G40">
         <v>458</v>
       </c>
       <c r="H40" t="s">
-        <v>349</v>
+        <v>437</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2604,19 +2910,19 @@
         <v>57</v>
       </c>
       <c r="D41" t="s">
-        <v>203</v>
+        <v>245</v>
       </c>
       <c r="E41" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F41" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G41">
         <v>911</v>
       </c>
       <c r="H41" t="s">
-        <v>349</v>
+        <v>437</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2630,19 +2936,19 @@
         <v>58</v>
       </c>
       <c r="D42" t="s">
-        <v>204</v>
+        <v>246</v>
       </c>
       <c r="E42" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F42" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G42">
         <v>3005</v>
       </c>
       <c r="H42" t="s">
-        <v>349</v>
+        <v>437</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2656,19 +2962,19 @@
         <v>59</v>
       </c>
       <c r="D43" t="s">
-        <v>205</v>
+        <v>247</v>
       </c>
       <c r="E43" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F43" t="s">
-        <v>323</v>
+        <v>408</v>
       </c>
       <c r="G43">
         <v>385</v>
       </c>
       <c r="H43" t="s">
-        <v>350</v>
+        <v>438</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2682,19 +2988,19 @@
         <v>60</v>
       </c>
       <c r="D44" t="s">
-        <v>206</v>
+        <v>248</v>
       </c>
       <c r="E44" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F44" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G44">
         <v>352</v>
       </c>
       <c r="H44" t="s">
-        <v>350</v>
+        <v>438</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2708,19 +3014,19 @@
         <v>61</v>
       </c>
       <c r="D45" t="s">
-        <v>207</v>
+        <v>249</v>
       </c>
       <c r="E45" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F45" t="s">
-        <v>321</v>
+        <v>406</v>
       </c>
       <c r="G45">
         <v>330</v>
       </c>
       <c r="H45" t="s">
-        <v>351</v>
+        <v>439</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2734,19 +3040,19 @@
         <v>62</v>
       </c>
       <c r="D46" t="s">
-        <v>208</v>
+        <v>250</v>
       </c>
       <c r="E46" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F46" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G46">
         <v>384</v>
       </c>
       <c r="H46" t="s">
-        <v>352</v>
+        <v>440</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2760,19 +3066,19 @@
         <v>63</v>
       </c>
       <c r="D47" t="s">
-        <v>209</v>
+        <v>251</v>
       </c>
       <c r="E47" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F47" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G47">
         <v>387</v>
       </c>
       <c r="H47" t="s">
-        <v>352</v>
+        <v>440</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2786,19 +3092,19 @@
         <v>64</v>
       </c>
       <c r="D48" t="s">
-        <v>210</v>
+        <v>252</v>
       </c>
       <c r="E48" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F48" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G48">
         <v>488</v>
       </c>
       <c r="H48" t="s">
-        <v>352</v>
+        <v>440</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2812,19 +3118,19 @@
         <v>65</v>
       </c>
       <c r="D49" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="E49" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F49" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G49">
         <v>345</v>
       </c>
       <c r="H49" t="s">
-        <v>353</v>
+        <v>441</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2838,19 +3144,19 @@
         <v>66</v>
       </c>
       <c r="D50" t="s">
-        <v>212</v>
+        <v>254</v>
       </c>
       <c r="E50" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F50" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G50">
         <v>203</v>
       </c>
       <c r="H50" t="s">
-        <v>353</v>
+        <v>441</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2864,19 +3170,19 @@
         <v>67</v>
       </c>
       <c r="D51" t="s">
-        <v>213</v>
+        <v>255</v>
       </c>
       <c r="E51" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F51" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G51">
         <v>769</v>
       </c>
       <c r="H51" t="s">
-        <v>353</v>
+        <v>441</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -2890,19 +3196,19 @@
         <v>68</v>
       </c>
       <c r="D52" t="s">
-        <v>214</v>
+        <v>256</v>
       </c>
       <c r="E52" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F52" t="s">
-        <v>313</v>
+        <v>398</v>
       </c>
       <c r="G52">
         <v>435</v>
       </c>
       <c r="H52" t="s">
-        <v>354</v>
+        <v>442</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -2916,19 +3222,19 @@
         <v>69</v>
       </c>
       <c r="D53" t="s">
-        <v>215</v>
+        <v>257</v>
       </c>
       <c r="E53" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F53" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G53">
         <v>617</v>
       </c>
       <c r="H53" t="s">
-        <v>354</v>
+        <v>442</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -2942,19 +3248,19 @@
         <v>70</v>
       </c>
       <c r="D54" t="s">
-        <v>216</v>
+        <v>258</v>
       </c>
       <c r="E54" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F54" t="s">
-        <v>313</v>
+        <v>398</v>
       </c>
       <c r="G54">
         <v>325</v>
       </c>
       <c r="H54" t="s">
-        <v>355</v>
+        <v>443</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -2968,19 +3274,19 @@
         <v>71</v>
       </c>
       <c r="D55" t="s">
-        <v>217</v>
+        <v>259</v>
       </c>
       <c r="E55" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F55" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G55">
         <v>1056</v>
       </c>
       <c r="H55" t="s">
-        <v>356</v>
+        <v>444</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2994,19 +3300,19 @@
         <v>72</v>
       </c>
       <c r="D56" t="s">
-        <v>218</v>
+        <v>260</v>
       </c>
       <c r="E56" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F56" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G56">
         <v>1478</v>
       </c>
       <c r="H56" t="s">
-        <v>356</v>
+        <v>444</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -3020,19 +3326,19 @@
         <v>73</v>
       </c>
       <c r="D57" t="s">
-        <v>219</v>
+        <v>261</v>
       </c>
       <c r="E57" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F57" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G57">
         <v>2594</v>
       </c>
       <c r="H57" t="s">
-        <v>356</v>
+        <v>444</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -3046,19 +3352,19 @@
         <v>74</v>
       </c>
       <c r="D58" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="E58" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F58" t="s">
-        <v>324</v>
+        <v>409</v>
       </c>
       <c r="G58">
         <v>721</v>
       </c>
       <c r="H58" t="s">
-        <v>357</v>
+        <v>445</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -3072,19 +3378,19 @@
         <v>75</v>
       </c>
       <c r="D59" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="E59" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F59" t="s">
-        <v>317</v>
+        <v>402</v>
       </c>
       <c r="G59">
         <v>765</v>
       </c>
       <c r="H59" t="s">
-        <v>357</v>
+        <v>445</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -3098,19 +3404,19 @@
         <v>76</v>
       </c>
       <c r="D60" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="E60" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F60" t="s">
-        <v>325</v>
+        <v>410</v>
       </c>
       <c r="G60">
         <v>1399</v>
       </c>
       <c r="H60" t="s">
-        <v>357</v>
+        <v>445</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -3124,19 +3430,19 @@
         <v>77</v>
       </c>
       <c r="D61" t="s">
-        <v>223</v>
+        <v>265</v>
       </c>
       <c r="E61" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F61" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G61">
         <v>617</v>
       </c>
       <c r="H61" t="s">
-        <v>358</v>
+        <v>446</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -3150,19 +3456,19 @@
         <v>78</v>
       </c>
       <c r="D62" t="s">
-        <v>224</v>
+        <v>266</v>
       </c>
       <c r="E62" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F62" t="s">
-        <v>313</v>
+        <v>398</v>
       </c>
       <c r="G62">
         <v>1072</v>
       </c>
       <c r="H62" t="s">
-        <v>358</v>
+        <v>446</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -3176,19 +3482,19 @@
         <v>79</v>
       </c>
       <c r="D63" t="s">
-        <v>225</v>
+        <v>267</v>
       </c>
       <c r="E63" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F63" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G63">
         <v>424</v>
       </c>
       <c r="H63" t="s">
-        <v>358</v>
+        <v>446</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -3202,19 +3508,19 @@
         <v>80</v>
       </c>
       <c r="D64" t="s">
-        <v>226</v>
+        <v>268</v>
       </c>
       <c r="E64" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F64" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G64">
         <v>1511</v>
       </c>
       <c r="H64" t="s">
-        <v>358</v>
+        <v>446</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -3228,19 +3534,19 @@
         <v>81</v>
       </c>
       <c r="D65" t="s">
-        <v>227</v>
+        <v>269</v>
       </c>
       <c r="E65" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F65" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G65">
         <v>342</v>
       </c>
       <c r="H65" t="s">
-        <v>359</v>
+        <v>447</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -3254,19 +3560,19 @@
         <v>82</v>
       </c>
       <c r="D66" t="s">
-        <v>228</v>
+        <v>270</v>
       </c>
       <c r="E66" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F66" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G66">
         <v>830</v>
       </c>
       <c r="H66" t="s">
-        <v>359</v>
+        <v>447</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -3280,19 +3586,19 @@
         <v>83</v>
       </c>
       <c r="D67" t="s">
-        <v>229</v>
+        <v>271</v>
       </c>
       <c r="E67" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F67" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G67">
         <v>1863</v>
       </c>
       <c r="H67" t="s">
-        <v>359</v>
+        <v>447</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -3306,19 +3612,19 @@
         <v>84</v>
       </c>
       <c r="D68" t="s">
-        <v>230</v>
+        <v>272</v>
       </c>
       <c r="E68" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F68" t="s">
-        <v>313</v>
+        <v>398</v>
       </c>
       <c r="G68">
         <v>1661</v>
       </c>
       <c r="H68" t="s">
-        <v>360</v>
+        <v>448</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -3332,19 +3638,19 @@
         <v>85</v>
       </c>
       <c r="D69" t="s">
-        <v>231</v>
+        <v>273</v>
       </c>
       <c r="E69" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F69" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G69">
         <v>1883</v>
       </c>
       <c r="H69" t="s">
-        <v>360</v>
+        <v>448</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -3358,19 +3664,19 @@
         <v>86</v>
       </c>
       <c r="D70" t="s">
-        <v>232</v>
+        <v>274</v>
       </c>
       <c r="E70" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F70" t="s">
-        <v>313</v>
+        <v>398</v>
       </c>
       <c r="G70">
         <v>1131</v>
       </c>
       <c r="H70" t="s">
-        <v>361</v>
+        <v>449</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -3384,19 +3690,19 @@
         <v>87</v>
       </c>
       <c r="D71" t="s">
-        <v>233</v>
+        <v>275</v>
       </c>
       <c r="E71" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F71" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G71">
         <v>511</v>
       </c>
       <c r="H71" t="s">
-        <v>361</v>
+        <v>449</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -3410,19 +3716,19 @@
         <v>88</v>
       </c>
       <c r="D72" t="s">
-        <v>234</v>
+        <v>276</v>
       </c>
       <c r="E72" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F72" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G72">
         <v>601</v>
       </c>
       <c r="H72" t="s">
-        <v>362</v>
+        <v>450</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3436,19 +3742,19 @@
         <v>89</v>
       </c>
       <c r="D73" t="s">
-        <v>235</v>
+        <v>277</v>
       </c>
       <c r="E73" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F73" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G73">
         <v>1089</v>
       </c>
       <c r="H73" t="s">
-        <v>362</v>
+        <v>450</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -3462,19 +3768,19 @@
         <v>90</v>
       </c>
       <c r="D74" t="s">
-        <v>236</v>
+        <v>278</v>
       </c>
       <c r="E74" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F74" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G74">
         <v>1681</v>
       </c>
       <c r="H74" t="s">
-        <v>362</v>
+        <v>450</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -3488,19 +3794,19 @@
         <v>91</v>
       </c>
       <c r="D75" t="s">
-        <v>237</v>
+        <v>279</v>
       </c>
       <c r="E75" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F75" t="s">
-        <v>321</v>
+        <v>406</v>
       </c>
       <c r="G75">
         <v>603</v>
       </c>
       <c r="H75" t="s">
-        <v>363</v>
+        <v>451</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -3514,19 +3820,19 @@
         <v>92</v>
       </c>
       <c r="D76" t="s">
-        <v>238</v>
+        <v>280</v>
       </c>
       <c r="E76" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F76" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G76">
         <v>679</v>
       </c>
       <c r="H76" t="s">
-        <v>363</v>
+        <v>451</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3540,19 +3846,19 @@
         <v>93</v>
       </c>
       <c r="D77" t="s">
-        <v>239</v>
+        <v>281</v>
       </c>
       <c r="E77" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F77" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G77">
         <v>1286</v>
       </c>
       <c r="H77" t="s">
-        <v>363</v>
+        <v>451</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -3566,19 +3872,19 @@
         <v>94</v>
       </c>
       <c r="D78" t="s">
-        <v>240</v>
+        <v>282</v>
       </c>
       <c r="E78" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F78" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G78">
         <v>986</v>
       </c>
       <c r="H78" t="s">
-        <v>364</v>
+        <v>452</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -3592,19 +3898,19 @@
         <v>95</v>
       </c>
       <c r="D79" t="s">
-        <v>241</v>
+        <v>283</v>
       </c>
       <c r="E79" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F79" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G79">
         <v>327</v>
       </c>
       <c r="H79" t="s">
-        <v>365</v>
+        <v>453</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3618,19 +3924,19 @@
         <v>96</v>
       </c>
       <c r="D80" t="s">
-        <v>242</v>
+        <v>284</v>
       </c>
       <c r="E80" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F80" t="s">
-        <v>322</v>
+        <v>407</v>
       </c>
       <c r="G80">
         <v>304</v>
       </c>
       <c r="H80" t="s">
-        <v>365</v>
+        <v>453</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -3644,19 +3950,19 @@
         <v>97</v>
       </c>
       <c r="D81" t="s">
-        <v>243</v>
+        <v>285</v>
       </c>
       <c r="E81" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F81" t="s">
-        <v>313</v>
+        <v>398</v>
       </c>
       <c r="G81">
         <v>105</v>
       </c>
       <c r="H81" t="s">
-        <v>366</v>
+        <v>454</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -3670,19 +3976,19 @@
         <v>98</v>
       </c>
       <c r="D82" t="s">
-        <v>244</v>
+        <v>286</v>
       </c>
       <c r="E82" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F82" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G82">
         <v>1151</v>
       </c>
       <c r="H82" t="s">
-        <v>366</v>
+        <v>454</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -3696,19 +4002,19 @@
         <v>99</v>
       </c>
       <c r="D83" t="s">
-        <v>245</v>
+        <v>287</v>
       </c>
       <c r="E83" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F83" t="s">
-        <v>324</v>
+        <v>409</v>
       </c>
       <c r="G83">
         <v>236</v>
       </c>
       <c r="H83" t="s">
-        <v>367</v>
+        <v>455</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -3722,19 +4028,19 @@
         <v>100</v>
       </c>
       <c r="D84" t="s">
-        <v>246</v>
+        <v>288</v>
       </c>
       <c r="E84" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F84" t="s">
-        <v>315</v>
+        <v>400</v>
       </c>
       <c r="G84">
         <v>458</v>
       </c>
       <c r="H84" t="s">
-        <v>368</v>
+        <v>456</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -3748,19 +4054,19 @@
         <v>101</v>
       </c>
       <c r="D85" t="s">
-        <v>247</v>
+        <v>289</v>
       </c>
       <c r="E85" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F85" t="s">
-        <v>319</v>
+        <v>404</v>
       </c>
       <c r="G85">
         <v>650</v>
       </c>
       <c r="H85" t="s">
-        <v>368</v>
+        <v>456</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -3774,19 +4080,19 @@
         <v>102</v>
       </c>
       <c r="D86" t="s">
-        <v>248</v>
+        <v>290</v>
       </c>
       <c r="E86" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F86" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G86">
         <v>913</v>
       </c>
       <c r="H86" t="s">
-        <v>368</v>
+        <v>456</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -3800,19 +4106,19 @@
         <v>103</v>
       </c>
       <c r="D87" t="s">
-        <v>249</v>
+        <v>291</v>
       </c>
       <c r="E87" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F87" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G87">
         <v>532</v>
       </c>
       <c r="H87" t="s">
-        <v>369</v>
+        <v>457</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -3826,19 +4132,19 @@
         <v>104</v>
       </c>
       <c r="D88" t="s">
-        <v>250</v>
+        <v>292</v>
       </c>
       <c r="E88" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F88" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G88">
         <v>547</v>
       </c>
       <c r="H88" t="s">
-        <v>369</v>
+        <v>457</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -3852,19 +4158,19 @@
         <v>105</v>
       </c>
       <c r="D89" t="s">
-        <v>251</v>
+        <v>293</v>
       </c>
       <c r="E89" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F89" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G89">
         <v>1003</v>
       </c>
       <c r="H89" t="s">
-        <v>369</v>
+        <v>457</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -3878,19 +4184,19 @@
         <v>106</v>
       </c>
       <c r="D90" t="s">
-        <v>252</v>
+        <v>294</v>
       </c>
       <c r="E90" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F90" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G90">
         <v>273</v>
       </c>
       <c r="H90" t="s">
-        <v>370</v>
+        <v>458</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -3904,19 +4210,19 @@
         <v>107</v>
       </c>
       <c r="D91" t="s">
-        <v>253</v>
+        <v>295</v>
       </c>
       <c r="E91" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F91" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G91">
         <v>1971</v>
       </c>
       <c r="H91" t="s">
-        <v>370</v>
+        <v>458</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -3930,19 +4236,19 @@
         <v>108</v>
       </c>
       <c r="D92" t="s">
-        <v>254</v>
+        <v>296</v>
       </c>
       <c r="E92" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F92" t="s">
-        <v>317</v>
+        <v>402</v>
       </c>
       <c r="G92">
         <v>681</v>
       </c>
       <c r="H92" t="s">
-        <v>371</v>
+        <v>459</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -3956,19 +4262,19 @@
         <v>109</v>
       </c>
       <c r="D93" t="s">
-        <v>255</v>
+        <v>297</v>
       </c>
       <c r="E93" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F93" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G93">
         <v>1238</v>
       </c>
       <c r="H93" t="s">
-        <v>371</v>
+        <v>459</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -3982,19 +4288,19 @@
         <v>110</v>
       </c>
       <c r="D94" t="s">
-        <v>256</v>
+        <v>298</v>
       </c>
       <c r="E94" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F94" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G94">
         <v>383</v>
       </c>
       <c r="H94" t="s">
-        <v>372</v>
+        <v>460</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -4008,19 +4314,19 @@
         <v>111</v>
       </c>
       <c r="D95" t="s">
-        <v>257</v>
+        <v>299</v>
       </c>
       <c r="E95" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F95" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G95">
         <v>1093</v>
       </c>
       <c r="H95" t="s">
-        <v>372</v>
+        <v>460</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -4034,19 +4340,19 @@
         <v>112</v>
       </c>
       <c r="D96" t="s">
-        <v>258</v>
+        <v>300</v>
       </c>
       <c r="E96" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F96" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G96">
         <v>1451</v>
       </c>
       <c r="H96" t="s">
-        <v>372</v>
+        <v>460</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -4060,19 +4366,19 @@
         <v>113</v>
       </c>
       <c r="D97" t="s">
-        <v>259</v>
+        <v>301</v>
       </c>
       <c r="E97" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F97" t="s">
-        <v>321</v>
+        <v>406</v>
       </c>
       <c r="G97">
         <v>577</v>
       </c>
       <c r="H97" t="s">
-        <v>373</v>
+        <v>461</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -4086,19 +4392,19 @@
         <v>114</v>
       </c>
       <c r="D98" t="s">
-        <v>260</v>
+        <v>302</v>
       </c>
       <c r="E98" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F98" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G98">
         <v>992</v>
       </c>
       <c r="H98" t="s">
-        <v>373</v>
+        <v>461</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -4112,19 +4418,19 @@
         <v>115</v>
       </c>
       <c r="D99" t="s">
-        <v>261</v>
+        <v>303</v>
       </c>
       <c r="E99" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F99" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G99">
         <v>1285</v>
       </c>
       <c r="H99" t="s">
-        <v>373</v>
+        <v>461</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -4138,19 +4444,19 @@
         <v>116</v>
       </c>
       <c r="D100" t="s">
-        <v>262</v>
+        <v>304</v>
       </c>
       <c r="E100" t="s">
-        <v>311</v>
+        <v>396</v>
       </c>
       <c r="F100" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G100">
         <v>466</v>
       </c>
       <c r="H100" t="s">
-        <v>374</v>
+        <v>462</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -4164,19 +4470,19 @@
         <v>117</v>
       </c>
       <c r="D101" t="s">
-        <v>263</v>
+        <v>305</v>
       </c>
       <c r="E101" t="s">
-        <v>311</v>
+        <v>396</v>
       </c>
       <c r="F101" t="s">
-        <v>326</v>
+        <v>411</v>
       </c>
       <c r="G101">
         <v>1761</v>
       </c>
       <c r="H101" t="s">
-        <v>374</v>
+        <v>462</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -4190,19 +4496,19 @@
         <v>118</v>
       </c>
       <c r="D102" t="s">
-        <v>264</v>
+        <v>306</v>
       </c>
       <c r="E102" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F102" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G102">
         <v>493</v>
       </c>
       <c r="H102" t="s">
-        <v>375</v>
+        <v>463</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -4216,19 +4522,19 @@
         <v>119</v>
       </c>
       <c r="D103" t="s">
-        <v>265</v>
+        <v>307</v>
       </c>
       <c r="E103" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F103" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G103">
         <v>604</v>
       </c>
       <c r="H103" t="s">
-        <v>375</v>
+        <v>463</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -4242,19 +4548,19 @@
         <v>120</v>
       </c>
       <c r="D104" t="s">
-        <v>266</v>
+        <v>308</v>
       </c>
       <c r="E104" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F104" t="s">
-        <v>327</v>
+        <v>412</v>
       </c>
       <c r="G104">
         <v>1107</v>
       </c>
       <c r="H104" t="s">
-        <v>375</v>
+        <v>463</v>
       </c>
     </row>
     <row r="105" spans="1:8">
@@ -4268,19 +4574,19 @@
         <v>121</v>
       </c>
       <c r="D105" t="s">
-        <v>267</v>
+        <v>309</v>
       </c>
       <c r="E105" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F105" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G105">
         <v>259</v>
       </c>
       <c r="H105" t="s">
-        <v>376</v>
+        <v>464</v>
       </c>
     </row>
     <row r="106" spans="1:8">
@@ -4294,19 +4600,19 @@
         <v>122</v>
       </c>
       <c r="D106" t="s">
-        <v>268</v>
+        <v>310</v>
       </c>
       <c r="E106" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F106" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G106">
         <v>615</v>
       </c>
       <c r="H106" t="s">
-        <v>376</v>
+        <v>464</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -4320,19 +4626,19 @@
         <v>123</v>
       </c>
       <c r="D107" t="s">
-        <v>269</v>
+        <v>311</v>
       </c>
       <c r="E107" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F107" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G107">
         <v>1390</v>
       </c>
       <c r="H107" t="s">
-        <v>376</v>
+        <v>464</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -4346,19 +4652,19 @@
         <v>124</v>
       </c>
       <c r="D108" t="s">
-        <v>270</v>
+        <v>312</v>
       </c>
       <c r="E108" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F108" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G108">
         <v>599</v>
       </c>
       <c r="H108" t="s">
-        <v>377</v>
+        <v>465</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -4372,19 +4678,19 @@
         <v>125</v>
       </c>
       <c r="D109" t="s">
-        <v>271</v>
+        <v>313</v>
       </c>
       <c r="E109" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F109" t="s">
-        <v>319</v>
+        <v>404</v>
       </c>
       <c r="G109">
         <v>739</v>
       </c>
       <c r="H109" t="s">
-        <v>377</v>
+        <v>465</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -4398,19 +4704,19 @@
         <v>126</v>
       </c>
       <c r="D110" t="s">
-        <v>272</v>
+        <v>314</v>
       </c>
       <c r="E110" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F110" t="s">
-        <v>327</v>
+        <v>412</v>
       </c>
       <c r="G110">
         <v>725</v>
       </c>
       <c r="H110" t="s">
-        <v>377</v>
+        <v>465</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -4424,19 +4730,19 @@
         <v>127</v>
       </c>
       <c r="D111" t="s">
-        <v>273</v>
+        <v>315</v>
       </c>
       <c r="E111" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F111" t="s">
-        <v>315</v>
+        <v>400</v>
       </c>
       <c r="G111">
         <v>1079</v>
       </c>
       <c r="H111" t="s">
-        <v>378</v>
+        <v>466</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -4450,19 +4756,19 @@
         <v>128</v>
       </c>
       <c r="D112" t="s">
-        <v>274</v>
+        <v>316</v>
       </c>
       <c r="E112" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F112" t="s">
-        <v>328</v>
+        <v>413</v>
       </c>
       <c r="G112">
         <v>779</v>
       </c>
       <c r="H112" t="s">
-        <v>378</v>
+        <v>466</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -4476,19 +4782,19 @@
         <v>129</v>
       </c>
       <c r="D113" t="s">
-        <v>275</v>
+        <v>317</v>
       </c>
       <c r="E113" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F113" t="s">
-        <v>327</v>
+        <v>412</v>
       </c>
       <c r="G113">
         <v>926</v>
       </c>
       <c r="H113" t="s">
-        <v>378</v>
+        <v>466</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -4502,19 +4808,19 @@
         <v>130</v>
       </c>
       <c r="D114" t="s">
-        <v>276</v>
+        <v>318</v>
       </c>
       <c r="E114" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F114" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G114">
         <v>878</v>
       </c>
       <c r="H114" t="s">
-        <v>379</v>
+        <v>467</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -4528,19 +4834,19 @@
         <v>131</v>
       </c>
       <c r="D115" t="s">
-        <v>277</v>
+        <v>319</v>
       </c>
       <c r="E115" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F115" t="s">
-        <v>327</v>
+        <v>412</v>
       </c>
       <c r="G115">
         <v>2025</v>
       </c>
       <c r="H115" t="s">
-        <v>379</v>
+        <v>467</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -4554,19 +4860,19 @@
         <v>132</v>
       </c>
       <c r="D116" t="s">
-        <v>278</v>
+        <v>320</v>
       </c>
       <c r="E116" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F116" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G116">
         <v>497</v>
       </c>
       <c r="H116" t="s">
-        <v>380</v>
+        <v>468</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -4580,19 +4886,19 @@
         <v>133</v>
       </c>
       <c r="D117" t="s">
-        <v>279</v>
+        <v>321</v>
       </c>
       <c r="E117" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F117" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G117">
         <v>363</v>
       </c>
       <c r="H117" t="s">
-        <v>380</v>
+        <v>468</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -4606,19 +4912,19 @@
         <v>134</v>
       </c>
       <c r="D118" t="s">
-        <v>280</v>
+        <v>322</v>
       </c>
       <c r="E118" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F118" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G118">
         <v>829</v>
       </c>
       <c r="H118" t="s">
-        <v>380</v>
+        <v>468</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -4632,19 +4938,19 @@
         <v>135</v>
       </c>
       <c r="D119" t="s">
-        <v>281</v>
+        <v>323</v>
       </c>
       <c r="E119" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F119" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G119">
         <v>766</v>
       </c>
       <c r="H119" t="s">
-        <v>381</v>
+        <v>469</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -4658,19 +4964,19 @@
         <v>136</v>
       </c>
       <c r="D120" t="s">
-        <v>282</v>
+        <v>324</v>
       </c>
       <c r="E120" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F120" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G120">
         <v>1068</v>
       </c>
       <c r="H120" t="s">
-        <v>381</v>
+        <v>469</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -4684,19 +4990,19 @@
         <v>137</v>
       </c>
       <c r="D121" t="s">
-        <v>283</v>
+        <v>325</v>
       </c>
       <c r="E121" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F121" t="s">
-        <v>328</v>
+        <v>413</v>
       </c>
       <c r="G121">
         <v>401</v>
       </c>
       <c r="H121" t="s">
-        <v>382</v>
+        <v>470</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -4710,19 +5016,19 @@
         <v>138</v>
       </c>
       <c r="D122" t="s">
-        <v>284</v>
+        <v>326</v>
       </c>
       <c r="E122" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F122" t="s">
-        <v>315</v>
+        <v>400</v>
       </c>
       <c r="G122">
         <v>540</v>
       </c>
       <c r="H122" t="s">
-        <v>382</v>
+        <v>470</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -4736,19 +5042,19 @@
         <v>139</v>
       </c>
       <c r="D123" t="s">
-        <v>285</v>
+        <v>327</v>
       </c>
       <c r="E123" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F123" t="s">
-        <v>327</v>
+        <v>412</v>
       </c>
       <c r="G123">
         <v>371</v>
       </c>
       <c r="H123" t="s">
-        <v>382</v>
+        <v>470</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -4762,19 +5068,19 @@
         <v>140</v>
       </c>
       <c r="D124" t="s">
-        <v>286</v>
+        <v>328</v>
       </c>
       <c r="E124" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F124" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G124">
         <v>549</v>
       </c>
       <c r="H124" t="s">
-        <v>383</v>
+        <v>471</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -4788,19 +5094,19 @@
         <v>141</v>
       </c>
       <c r="D125" t="s">
-        <v>287</v>
+        <v>329</v>
       </c>
       <c r="E125" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F125" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G125">
         <v>656</v>
       </c>
       <c r="H125" t="s">
-        <v>383</v>
+        <v>471</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -4814,19 +5120,19 @@
         <v>142</v>
       </c>
       <c r="D126" t="s">
-        <v>288</v>
+        <v>330</v>
       </c>
       <c r="E126" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F126" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G126">
         <v>1980</v>
       </c>
       <c r="H126" t="s">
-        <v>383</v>
+        <v>471</v>
       </c>
     </row>
     <row r="127" spans="1:8">
@@ -4840,19 +5146,19 @@
         <v>143</v>
       </c>
       <c r="D127" t="s">
-        <v>289</v>
+        <v>331</v>
       </c>
       <c r="E127" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F127" t="s">
-        <v>329</v>
+        <v>414</v>
       </c>
       <c r="G127">
         <v>585</v>
       </c>
       <c r="H127" t="s">
-        <v>384</v>
+        <v>472</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -4866,19 +5172,19 @@
         <v>144</v>
       </c>
       <c r="D128" t="s">
-        <v>290</v>
+        <v>332</v>
       </c>
       <c r="E128" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F128" t="s">
-        <v>327</v>
+        <v>412</v>
       </c>
       <c r="G128">
         <v>1459</v>
       </c>
       <c r="H128" t="s">
-        <v>384</v>
+        <v>472</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -4892,19 +5198,19 @@
         <v>145</v>
       </c>
       <c r="D129" t="s">
-        <v>291</v>
+        <v>333</v>
       </c>
       <c r="E129" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F129" t="s">
-        <v>324</v>
+        <v>409</v>
       </c>
       <c r="G129">
         <v>420</v>
       </c>
       <c r="H129" t="s">
-        <v>385</v>
+        <v>473</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -4918,19 +5224,19 @@
         <v>146</v>
       </c>
       <c r="D130" t="s">
-        <v>292</v>
+        <v>334</v>
       </c>
       <c r="E130" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F130" t="s">
-        <v>330</v>
+        <v>415</v>
       </c>
       <c r="G130">
         <v>686</v>
       </c>
       <c r="H130" t="s">
-        <v>385</v>
+        <v>473</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -4944,19 +5250,19 @@
         <v>147</v>
       </c>
       <c r="D131" t="s">
-        <v>293</v>
+        <v>335</v>
       </c>
       <c r="E131" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F131" t="s">
-        <v>331</v>
+        <v>416</v>
       </c>
       <c r="G131">
         <v>1604</v>
       </c>
       <c r="H131" t="s">
-        <v>385</v>
+        <v>473</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -4970,19 +5276,19 @@
         <v>148</v>
       </c>
       <c r="D132" t="s">
-        <v>294</v>
+        <v>336</v>
       </c>
       <c r="E132" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F132" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="G132">
         <v>508</v>
       </c>
       <c r="H132" t="s">
-        <v>386</v>
+        <v>474</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -4996,19 +5302,19 @@
         <v>149</v>
       </c>
       <c r="D133" t="s">
-        <v>295</v>
+        <v>337</v>
       </c>
       <c r="E133" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F133" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G133">
         <v>938</v>
       </c>
       <c r="H133" t="s">
-        <v>386</v>
+        <v>474</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -5022,19 +5328,19 @@
         <v>150</v>
       </c>
       <c r="D134" t="s">
-        <v>296</v>
+        <v>338</v>
       </c>
       <c r="E134" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F134" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G134">
         <v>1142</v>
       </c>
       <c r="H134" t="s">
-        <v>386</v>
+        <v>474</v>
       </c>
     </row>
     <row r="135" spans="1:8">
@@ -5048,19 +5354,19 @@
         <v>151</v>
       </c>
       <c r="D135" t="s">
-        <v>297</v>
+        <v>339</v>
       </c>
       <c r="E135" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F135" t="s">
-        <v>326</v>
+        <v>411</v>
       </c>
       <c r="G135">
         <v>500</v>
       </c>
       <c r="H135" t="s">
-        <v>387</v>
+        <v>475</v>
       </c>
     </row>
     <row r="136" spans="1:8">
@@ -5074,19 +5380,19 @@
         <v>152</v>
       </c>
       <c r="D136" t="s">
-        <v>298</v>
+        <v>340</v>
       </c>
       <c r="E136" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F136" t="s">
-        <v>332</v>
+        <v>417</v>
       </c>
       <c r="G136">
         <v>704</v>
       </c>
       <c r="H136" t="s">
-        <v>387</v>
+        <v>475</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -5100,19 +5406,19 @@
         <v>153</v>
       </c>
       <c r="D137" t="s">
-        <v>299</v>
+        <v>341</v>
       </c>
       <c r="E137" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F137" t="s">
-        <v>333</v>
+        <v>418</v>
       </c>
       <c r="G137">
         <v>737</v>
       </c>
       <c r="H137" t="s">
-        <v>387</v>
+        <v>475</v>
       </c>
     </row>
     <row r="138" spans="1:8">
@@ -5126,19 +5432,19 @@
         <v>154</v>
       </c>
       <c r="D138" t="s">
-        <v>300</v>
+        <v>342</v>
       </c>
       <c r="E138" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F138" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G138">
         <v>1841</v>
       </c>
       <c r="H138" t="s">
-        <v>387</v>
+        <v>475</v>
       </c>
     </row>
     <row r="139" spans="1:8">
@@ -5152,19 +5458,19 @@
         <v>155</v>
       </c>
       <c r="D139" t="s">
-        <v>301</v>
+        <v>343</v>
       </c>
       <c r="E139" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F139" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G139">
         <v>233</v>
       </c>
       <c r="H139" t="s">
-        <v>388</v>
+        <v>476</v>
       </c>
     </row>
     <row r="140" spans="1:8">
@@ -5178,19 +5484,19 @@
         <v>156</v>
       </c>
       <c r="D140" t="s">
-        <v>302</v>
+        <v>344</v>
       </c>
       <c r="E140" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F140" t="s">
-        <v>320</v>
+        <v>405</v>
       </c>
       <c r="G140">
         <v>318</v>
       </c>
       <c r="H140" t="s">
-        <v>389</v>
+        <v>477</v>
       </c>
     </row>
     <row r="141" spans="1:8">
@@ -5204,19 +5510,19 @@
         <v>157</v>
       </c>
       <c r="D141" t="s">
-        <v>303</v>
+        <v>345</v>
       </c>
       <c r="E141" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F141" t="s">
-        <v>327</v>
+        <v>412</v>
       </c>
       <c r="G141">
         <v>1692</v>
       </c>
       <c r="H141" t="s">
-        <v>389</v>
+        <v>477</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -5230,19 +5536,19 @@
         <v>158</v>
       </c>
       <c r="D142" t="s">
-        <v>304</v>
+        <v>346</v>
       </c>
       <c r="E142" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F142" t="s">
-        <v>321</v>
+        <v>406</v>
       </c>
       <c r="G142">
         <v>766</v>
       </c>
       <c r="H142" t="s">
-        <v>390</v>
+        <v>478</v>
       </c>
     </row>
     <row r="143" spans="1:8">
@@ -5256,19 +5562,19 @@
         <v>159</v>
       </c>
       <c r="D143" t="s">
-        <v>305</v>
+        <v>347</v>
       </c>
       <c r="E143" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F143" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G143">
         <v>843</v>
       </c>
       <c r="H143" t="s">
-        <v>390</v>
+        <v>478</v>
       </c>
     </row>
     <row r="144" spans="1:8">
@@ -5282,19 +5588,19 @@
         <v>160</v>
       </c>
       <c r="D144" t="s">
-        <v>306</v>
+        <v>348</v>
       </c>
       <c r="E144" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F144" t="s">
-        <v>313</v>
+        <v>398</v>
       </c>
       <c r="G144">
         <v>651</v>
       </c>
       <c r="H144" t="s">
-        <v>391</v>
+        <v>479</v>
       </c>
     </row>
     <row r="145" spans="1:8">
@@ -5308,19 +5614,19 @@
         <v>161</v>
       </c>
       <c r="D145" t="s">
-        <v>307</v>
+        <v>349</v>
       </c>
       <c r="E145" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F145" t="s">
-        <v>321</v>
+        <v>406</v>
       </c>
       <c r="G145">
         <v>665</v>
       </c>
       <c r="H145" t="s">
-        <v>392</v>
+        <v>480</v>
       </c>
     </row>
     <row r="146" spans="1:8">
@@ -5334,19 +5640,19 @@
         <v>162</v>
       </c>
       <c r="D146" t="s">
-        <v>308</v>
+        <v>350</v>
       </c>
       <c r="E146" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F146" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="G146">
         <v>952</v>
       </c>
       <c r="H146" t="s">
-        <v>392</v>
+        <v>480</v>
       </c>
     </row>
     <row r="147" spans="1:8">
@@ -5360,19 +5666,1137 @@
         <v>163</v>
       </c>
       <c r="D147" t="s">
-        <v>309</v>
+        <v>351</v>
       </c>
       <c r="E147" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="F147" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="G147">
         <v>1336</v>
       </c>
       <c r="H147" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8">
+      <c r="A148" s="1">
+        <v>146</v>
+      </c>
+      <c r="B148" t="s">
+        <v>13</v>
+      </c>
+      <c r="C148" t="s">
+        <v>164</v>
+      </c>
+      <c r="D148" t="s">
+        <v>352</v>
+      </c>
+      <c r="E148" t="s">
+        <v>395</v>
+      </c>
+      <c r="F148" t="s">
+        <v>406</v>
+      </c>
+      <c r="G148">
+        <v>587</v>
+      </c>
+      <c r="H148" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8">
+      <c r="A149" s="1">
+        <v>147</v>
+      </c>
+      <c r="B149" t="s">
+        <v>8</v>
+      </c>
+      <c r="C149" t="s">
+        <v>165</v>
+      </c>
+      <c r="D149" t="s">
+        <v>353</v>
+      </c>
+      <c r="E149" t="s">
+        <v>395</v>
+      </c>
+      <c r="F149" t="s">
+        <v>403</v>
+      </c>
+      <c r="G149">
+        <v>569</v>
+      </c>
+      <c r="H149" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8">
+      <c r="A150" s="1">
+        <v>148</v>
+      </c>
+      <c r="B150" t="s">
+        <v>13</v>
+      </c>
+      <c r="C150" t="s">
+        <v>166</v>
+      </c>
+      <c r="D150" t="s">
+        <v>354</v>
+      </c>
+      <c r="E150" t="s">
+        <v>395</v>
+      </c>
+      <c r="F150" t="s">
+        <v>399</v>
+      </c>
+      <c r="G150">
+        <v>1292</v>
+      </c>
+      <c r="H150" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8">
+      <c r="A151" s="1">
+        <v>149</v>
+      </c>
+      <c r="B151" t="s">
+        <v>10</v>
+      </c>
+      <c r="C151" t="s">
+        <v>167</v>
+      </c>
+      <c r="D151" t="s">
+        <v>355</v>
+      </c>
+      <c r="E151" t="s">
+        <v>395</v>
+      </c>
+      <c r="F151" t="s">
+        <v>406</v>
+      </c>
+      <c r="G151">
+        <v>435</v>
+      </c>
+      <c r="H151" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8">
+      <c r="A152" s="1">
+        <v>150</v>
+      </c>
+      <c r="B152" t="s">
+        <v>13</v>
+      </c>
+      <c r="C152" t="s">
+        <v>168</v>
+      </c>
+      <c r="D152" t="s">
+        <v>356</v>
+      </c>
+      <c r="E152" t="s">
+        <v>395</v>
+      </c>
+      <c r="F152" t="s">
+        <v>403</v>
+      </c>
+      <c r="G152">
+        <v>962</v>
+      </c>
+      <c r="H152" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8">
+      <c r="A153" s="1">
+        <v>151</v>
+      </c>
+      <c r="B153" t="s">
+        <v>10</v>
+      </c>
+      <c r="C153" t="s">
+        <v>169</v>
+      </c>
+      <c r="D153" t="s">
+        <v>357</v>
+      </c>
+      <c r="E153" t="s">
+        <v>395</v>
+      </c>
+      <c r="F153" t="s">
+        <v>399</v>
+      </c>
+      <c r="G153">
+        <v>1077</v>
+      </c>
+      <c r="H153" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8">
+      <c r="A154" s="1">
+        <v>152</v>
+      </c>
+      <c r="B154" t="s">
+        <v>9</v>
+      </c>
+      <c r="C154" t="s">
+        <v>170</v>
+      </c>
+      <c r="D154" t="s">
+        <v>358</v>
+      </c>
+      <c r="E154" t="s">
+        <v>395</v>
+      </c>
+      <c r="F154" t="s">
+        <v>419</v>
+      </c>
+      <c r="G154">
+        <v>300</v>
+      </c>
+      <c r="H154" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8">
+      <c r="A155" s="1">
+        <v>153</v>
+      </c>
+      <c r="B155" t="s">
+        <v>9</v>
+      </c>
+      <c r="C155" t="s">
+        <v>171</v>
+      </c>
+      <c r="D155" t="s">
+        <v>359</v>
+      </c>
+      <c r="E155" t="s">
+        <v>395</v>
+      </c>
+      <c r="F155" t="s">
+        <v>413</v>
+      </c>
+      <c r="G155">
+        <v>380</v>
+      </c>
+      <c r="H155" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8">
+      <c r="A156" s="1">
+        <v>154</v>
+      </c>
+      <c r="B156" t="s">
+        <v>15</v>
+      </c>
+      <c r="C156" t="s">
+        <v>172</v>
+      </c>
+      <c r="D156" t="s">
+        <v>360</v>
+      </c>
+      <c r="E156" t="s">
+        <v>395</v>
+      </c>
+      <c r="F156" t="s">
+        <v>399</v>
+      </c>
+      <c r="G156">
+        <v>311</v>
+      </c>
+      <c r="H156" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8">
+      <c r="A157" s="1">
+        <v>155</v>
+      </c>
+      <c r="B157" t="s">
+        <v>14</v>
+      </c>
+      <c r="C157" t="s">
+        <v>167</v>
+      </c>
+      <c r="D157" t="s">
+        <v>361</v>
+      </c>
+      <c r="E157" t="s">
+        <v>395</v>
+      </c>
+      <c r="F157" t="s">
+        <v>400</v>
+      </c>
+      <c r="G157">
+        <v>598</v>
+      </c>
+      <c r="H157" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8">
+      <c r="A158" s="1">
+        <v>156</v>
+      </c>
+      <c r="B158" t="s">
+        <v>10</v>
+      </c>
+      <c r="C158" t="s">
+        <v>173</v>
+      </c>
+      <c r="D158" t="s">
+        <v>362</v>
+      </c>
+      <c r="E158" t="s">
+        <v>395</v>
+      </c>
+      <c r="F158" t="s">
+        <v>403</v>
+      </c>
+      <c r="G158">
+        <v>666</v>
+      </c>
+      <c r="H158" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8">
+      <c r="A159" s="1">
+        <v>157</v>
+      </c>
+      <c r="B159" t="s">
+        <v>13</v>
+      </c>
+      <c r="C159" t="s">
+        <v>174</v>
+      </c>
+      <c r="D159" t="s">
+        <v>363</v>
+      </c>
+      <c r="E159" t="s">
+        <v>395</v>
+      </c>
+      <c r="F159" t="s">
+        <v>399</v>
+      </c>
+      <c r="G159">
+        <v>2207</v>
+      </c>
+      <c r="H159" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8">
+      <c r="A160" s="1">
+        <v>158</v>
+      </c>
+      <c r="B160" t="s">
+        <v>11</v>
+      </c>
+      <c r="C160" t="s">
+        <v>175</v>
+      </c>
+      <c r="D160" t="s">
+        <v>364</v>
+      </c>
+      <c r="E160" t="s">
+        <v>395</v>
+      </c>
+      <c r="F160" t="s">
+        <v>397</v>
+      </c>
+      <c r="G160">
+        <v>648</v>
+      </c>
+      <c r="H160" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8">
+      <c r="A161" s="1">
+        <v>159</v>
+      </c>
+      <c r="B161" t="s">
+        <v>10</v>
+      </c>
+      <c r="C161" t="s">
+        <v>176</v>
+      </c>
+      <c r="D161" t="s">
+        <v>365</v>
+      </c>
+      <c r="E161" t="s">
+        <v>395</v>
+      </c>
+      <c r="F161" t="s">
+        <v>403</v>
+      </c>
+      <c r="G161">
+        <v>812</v>
+      </c>
+      <c r="H161" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8">
+      <c r="A162" s="1">
+        <v>160</v>
+      </c>
+      <c r="B162" t="s">
+        <v>15</v>
+      </c>
+      <c r="C162" t="s">
+        <v>177</v>
+      </c>
+      <c r="D162" t="s">
+        <v>366</v>
+      </c>
+      <c r="E162" t="s">
+        <v>395</v>
+      </c>
+      <c r="F162" t="s">
+        <v>399</v>
+      </c>
+      <c r="G162">
+        <v>1633</v>
+      </c>
+      <c r="H162" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8">
+      <c r="A163" s="1">
+        <v>161</v>
+      </c>
+      <c r="B163" t="s">
+        <v>10</v>
+      </c>
+      <c r="C163" t="s">
+        <v>178</v>
+      </c>
+      <c r="D163" t="s">
+        <v>367</v>
+      </c>
+      <c r="E163" t="s">
+        <v>395</v>
+      </c>
+      <c r="F163" t="s">
+        <v>397</v>
+      </c>
+      <c r="G163">
+        <v>704</v>
+      </c>
+      <c r="H163" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8">
+      <c r="A164" s="1">
+        <v>162</v>
+      </c>
+      <c r="B164" t="s">
+        <v>10</v>
+      </c>
+      <c r="C164" t="s">
+        <v>179</v>
+      </c>
+      <c r="D164" t="s">
+        <v>368</v>
+      </c>
+      <c r="E164" t="s">
+        <v>395</v>
+      </c>
+      <c r="F164" t="s">
+        <v>403</v>
+      </c>
+      <c r="G164">
+        <v>860</v>
+      </c>
+      <c r="H164" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8">
+      <c r="A165" s="1">
+        <v>163</v>
+      </c>
+      <c r="B165" t="s">
+        <v>8</v>
+      </c>
+      <c r="C165" t="s">
+        <v>180</v>
+      </c>
+      <c r="D165" t="s">
+        <v>369</v>
+      </c>
+      <c r="E165" t="s">
+        <v>395</v>
+      </c>
+      <c r="F165" t="s">
+        <v>399</v>
+      </c>
+      <c r="G165">
+        <v>1826</v>
+      </c>
+      <c r="H165" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8">
+      <c r="A166" s="1">
+        <v>164</v>
+      </c>
+      <c r="B166" t="s">
+        <v>10</v>
+      </c>
+      <c r="C166" t="s">
+        <v>181</v>
+      </c>
+      <c r="D166" t="s">
+        <v>370</v>
+      </c>
+      <c r="E166" t="s">
+        <v>395</v>
+      </c>
+      <c r="F166" t="s">
+        <v>397</v>
+      </c>
+      <c r="G166">
+        <v>541</v>
+      </c>
+      <c r="H166" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8">
+      <c r="A167" s="1">
+        <v>165</v>
+      </c>
+      <c r="B167" t="s">
+        <v>13</v>
+      </c>
+      <c r="C167" t="s">
+        <v>182</v>
+      </c>
+      <c r="D167" t="s">
+        <v>371</v>
+      </c>
+      <c r="E167" t="s">
+        <v>395</v>
+      </c>
+      <c r="F167" t="s">
+        <v>403</v>
+      </c>
+      <c r="G167">
+        <v>764</v>
+      </c>
+      <c r="H167" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8">
+      <c r="A168" s="1">
+        <v>166</v>
+      </c>
+      <c r="B168" t="s">
+        <v>15</v>
+      </c>
+      <c r="C168" t="s">
+        <v>183</v>
+      </c>
+      <c r="D168" t="s">
+        <v>372</v>
+      </c>
+      <c r="E168" t="s">
+        <v>395</v>
+      </c>
+      <c r="F168" t="s">
+        <v>399</v>
+      </c>
+      <c r="G168">
+        <v>1536</v>
+      </c>
+      <c r="H168" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8">
+      <c r="A169" s="1">
+        <v>167</v>
+      </c>
+      <c r="B169" t="s">
+        <v>15</v>
+      </c>
+      <c r="C169" t="s">
+        <v>184</v>
+      </c>
+      <c r="D169" t="s">
+        <v>373</v>
+      </c>
+      <c r="E169" t="s">
+        <v>395</v>
+      </c>
+      <c r="F169" t="s">
+        <v>397</v>
+      </c>
+      <c r="G169">
+        <v>537</v>
+      </c>
+      <c r="H169" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8">
+      <c r="A170" s="1">
+        <v>168</v>
+      </c>
+      <c r="B170" t="s">
+        <v>13</v>
+      </c>
+      <c r="C170" t="s">
+        <v>185</v>
+      </c>
+      <c r="D170" t="s">
+        <v>374</v>
+      </c>
+      <c r="E170" t="s">
+        <v>395</v>
+      </c>
+      <c r="F170" t="s">
+        <v>403</v>
+      </c>
+      <c r="G170">
+        <v>588</v>
+      </c>
+      <c r="H170" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8">
+      <c r="A171" s="1">
+        <v>169</v>
+      </c>
+      <c r="B171" t="s">
+        <v>8</v>
+      </c>
+      <c r="C171" t="s">
+        <v>186</v>
+      </c>
+      <c r="D171" t="s">
+        <v>375</v>
+      </c>
+      <c r="E171" t="s">
+        <v>395</v>
+      </c>
+      <c r="F171" t="s">
+        <v>399</v>
+      </c>
+      <c r="G171">
+        <v>1370</v>
+      </c>
+      <c r="H171" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8">
+      <c r="A172" s="1">
+        <v>170</v>
+      </c>
+      <c r="B172" t="s">
+        <v>11</v>
+      </c>
+      <c r="C172" t="s">
+        <v>187</v>
+      </c>
+      <c r="D172" t="s">
+        <v>376</v>
+      </c>
+      <c r="E172" t="s">
+        <v>395</v>
+      </c>
+      <c r="F172" t="s">
+        <v>406</v>
+      </c>
+      <c r="G172">
+        <v>393</v>
+      </c>
+      <c r="H172" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8">
+      <c r="A173" s="1">
+        <v>171</v>
+      </c>
+      <c r="B173" t="s">
+        <v>13</v>
+      </c>
+      <c r="C173" t="s">
+        <v>188</v>
+      </c>
+      <c r="D173" t="s">
+        <v>377</v>
+      </c>
+      <c r="E173" t="s">
+        <v>395</v>
+      </c>
+      <c r="F173" t="s">
+        <v>403</v>
+      </c>
+      <c r="G173">
+        <v>593</v>
+      </c>
+      <c r="H173" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8">
+      <c r="A174" s="1">
+        <v>172</v>
+      </c>
+      <c r="B174" t="s">
+        <v>8</v>
+      </c>
+      <c r="C174" t="s">
+        <v>189</v>
+      </c>
+      <c r="D174" t="s">
+        <v>378</v>
+      </c>
+      <c r="E174" t="s">
+        <v>395</v>
+      </c>
+      <c r="F174" t="s">
+        <v>399</v>
+      </c>
+      <c r="G174">
+        <v>1085</v>
+      </c>
+      <c r="H174" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8">
+      <c r="A175" s="1">
+        <v>173</v>
+      </c>
+      <c r="B175" t="s">
+        <v>9</v>
+      </c>
+      <c r="C175" t="s">
+        <v>190</v>
+      </c>
+      <c r="D175" t="s">
+        <v>379</v>
+      </c>
+      <c r="E175" t="s">
+        <v>395</v>
+      </c>
+      <c r="F175" t="s">
+        <v>409</v>
+      </c>
+      <c r="G175">
+        <v>900</v>
+      </c>
+      <c r="H175" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8">
+      <c r="A176" s="1">
+        <v>174</v>
+      </c>
+      <c r="B176" t="s">
+        <v>9</v>
+      </c>
+      <c r="C176" t="s">
+        <v>191</v>
+      </c>
+      <c r="D176" t="s">
+        <v>380</v>
+      </c>
+      <c r="E176" t="s">
+        <v>395</v>
+      </c>
+      <c r="F176" t="s">
+        <v>402</v>
+      </c>
+      <c r="G176">
+        <v>470</v>
+      </c>
+      <c r="H176" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8">
+      <c r="A177" s="1">
+        <v>175</v>
+      </c>
+      <c r="B177" t="s">
+        <v>9</v>
+      </c>
+      <c r="C177" t="s">
+        <v>192</v>
+      </c>
+      <c r="D177" t="s">
+        <v>381</v>
+      </c>
+      <c r="E177" t="s">
+        <v>395</v>
+      </c>
+      <c r="F177" t="s">
+        <v>399</v>
+      </c>
+      <c r="G177">
+        <v>1079</v>
+      </c>
+      <c r="H177" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8">
+      <c r="A178" s="1">
+        <v>176</v>
+      </c>
+      <c r="B178" t="s">
+        <v>9</v>
+      </c>
+      <c r="C178" t="s">
+        <v>193</v>
+      </c>
+      <c r="D178" t="s">
+        <v>382</v>
+      </c>
+      <c r="E178" t="s">
+        <v>395</v>
+      </c>
+      <c r="F178" t="s">
+        <v>405</v>
+      </c>
+      <c r="G178">
+        <v>293</v>
+      </c>
+      <c r="H178" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8">
+      <c r="A179" s="1">
+        <v>177</v>
+      </c>
+      <c r="B179" t="s">
+        <v>15</v>
+      </c>
+      <c r="C179" t="s">
+        <v>194</v>
+      </c>
+      <c r="D179" t="s">
+        <v>383</v>
+      </c>
+      <c r="E179" t="s">
+        <v>395</v>
+      </c>
+      <c r="F179" t="s">
+        <v>402</v>
+      </c>
+      <c r="G179">
+        <v>380</v>
+      </c>
+      <c r="H179" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8">
+      <c r="A180" s="1">
+        <v>178</v>
+      </c>
+      <c r="B180" t="s">
+        <v>8</v>
+      </c>
+      <c r="C180" t="s">
+        <v>195</v>
+      </c>
+      <c r="D180" t="s">
+        <v>384</v>
+      </c>
+      <c r="E180" t="s">
+        <v>395</v>
+      </c>
+      <c r="F180" t="s">
+        <v>399</v>
+      </c>
+      <c r="G180">
+        <v>1013</v>
+      </c>
+      <c r="H180" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8">
+      <c r="A181" s="1">
+        <v>179</v>
+      </c>
+      <c r="B181" t="s">
+        <v>11</v>
+      </c>
+      <c r="C181" t="s">
+        <v>196</v>
+      </c>
+      <c r="D181" t="s">
+        <v>385</v>
+      </c>
+      <c r="E181" t="s">
+        <v>395</v>
+      </c>
+      <c r="F181" t="s">
+        <v>397</v>
+      </c>
+      <c r="G181">
+        <v>511</v>
+      </c>
+      <c r="H181" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8">
+      <c r="A182" s="1">
+        <v>180</v>
+      </c>
+      <c r="B182" t="s">
+        <v>10</v>
+      </c>
+      <c r="C182" t="s">
+        <v>197</v>
+      </c>
+      <c r="D182" t="s">
+        <v>386</v>
+      </c>
+      <c r="E182" t="s">
+        <v>395</v>
+      </c>
+      <c r="F182" t="s">
+        <v>403</v>
+      </c>
+      <c r="G182">
+        <v>647</v>
+      </c>
+      <c r="H182" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8">
+      <c r="A183" s="1">
+        <v>181</v>
+      </c>
+      <c r="B183" t="s">
+        <v>8</v>
+      </c>
+      <c r="C183" t="s">
+        <v>198</v>
+      </c>
+      <c r="D183" t="s">
+        <v>387</v>
+      </c>
+      <c r="E183" t="s">
+        <v>395</v>
+      </c>
+      <c r="F183" t="s">
+        <v>399</v>
+      </c>
+      <c r="G183">
+        <v>1054</v>
+      </c>
+      <c r="H183" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8">
+      <c r="A184" s="1">
+        <v>182</v>
+      </c>
+      <c r="B184" t="s">
+        <v>14</v>
+      </c>
+      <c r="C184" t="s">
+        <v>199</v>
+      </c>
+      <c r="D184" t="s">
+        <v>388</v>
+      </c>
+      <c r="E184" t="s">
+        <v>395</v>
+      </c>
+      <c r="F184" t="s">
+        <v>420</v>
+      </c>
+      <c r="G184">
+        <v>376</v>
+      </c>
+      <c r="H184" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8">
+      <c r="A185" s="1">
+        <v>183</v>
+      </c>
+      <c r="B185" t="s">
+        <v>10</v>
+      </c>
+      <c r="C185" t="s">
+        <v>200</v>
+      </c>
+      <c r="D185" t="s">
+        <v>389</v>
+      </c>
+      <c r="E185" t="s">
+        <v>395</v>
+      </c>
+      <c r="F185" t="s">
+        <v>403</v>
+      </c>
+      <c r="G185">
+        <v>344</v>
+      </c>
+      <c r="H185" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8">
+      <c r="A186" s="1">
+        <v>184</v>
+      </c>
+      <c r="B186" t="s">
+        <v>10</v>
+      </c>
+      <c r="C186" t="s">
+        <v>201</v>
+      </c>
+      <c r="D186" t="s">
+        <v>390</v>
+      </c>
+      <c r="E186" t="s">
+        <v>395</v>
+      </c>
+      <c r="F186" t="s">
+        <v>399</v>
+      </c>
+      <c r="G186">
+        <v>453</v>
+      </c>
+      <c r="H186" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8">
+      <c r="A187" s="1">
+        <v>185</v>
+      </c>
+      <c r="B187" t="s">
+        <v>15</v>
+      </c>
+      <c r="C187" t="s">
+        <v>202</v>
+      </c>
+      <c r="D187" t="s">
+        <v>391</v>
+      </c>
+      <c r="E187" t="s">
+        <v>395</v>
+      </c>
+      <c r="F187" t="s">
+        <v>421</v>
+      </c>
+      <c r="G187">
+        <v>516</v>
+      </c>
+      <c r="H187" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8">
+      <c r="A188" s="1">
+        <v>186</v>
+      </c>
+      <c r="B188" t="s">
+        <v>10</v>
+      </c>
+      <c r="C188" t="s">
+        <v>203</v>
+      </c>
+      <c r="D188" t="s">
         <v>392</v>
+      </c>
+      <c r="E188" t="s">
+        <v>395</v>
+      </c>
+      <c r="F188" t="s">
+        <v>401</v>
+      </c>
+      <c r="G188">
+        <v>604</v>
+      </c>
+      <c r="H188" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8">
+      <c r="A189" s="1">
+        <v>187</v>
+      </c>
+      <c r="B189" t="s">
+        <v>13</v>
+      </c>
+      <c r="C189" t="s">
+        <v>204</v>
+      </c>
+      <c r="D189" t="s">
+        <v>393</v>
+      </c>
+      <c r="E189" t="s">
+        <v>395</v>
+      </c>
+      <c r="F189" t="s">
+        <v>402</v>
+      </c>
+      <c r="G189">
+        <v>583</v>
+      </c>
+      <c r="H189" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8">
+      <c r="A190" s="1">
+        <v>188</v>
+      </c>
+      <c r="B190" t="s">
+        <v>13</v>
+      </c>
+      <c r="C190" t="s">
+        <v>205</v>
+      </c>
+      <c r="D190" t="s">
+        <v>394</v>
+      </c>
+      <c r="E190" t="s">
+        <v>395</v>
+      </c>
+      <c r="F190" t="s">
+        <v>399</v>
+      </c>
+      <c r="G190">
+        <v>901</v>
+      </c>
+      <c r="H190" t="s">
+        <v>494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>